<commit_message>
Add another sheet to keywords.xlsx with 17 Guatemala's municipios
</commit_message>
<xml_diff>
--- a/key_words.xlsx
+++ b/key_words.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAV\Documents\Python\Python_Project\House_price_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ECED0789-527A-40B7-BC41-52175A9F6C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA2CAC2-E2D4-4189-8415-283D81E65859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{463692C9-9AB7-487F-819A-911864E4C9A8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{463692C9-9AB7-487F-819A-911864E4C9A8}"/>
   </bookViews>
   <sheets>
     <sheet name="keywords" sheetId="1" r:id="rId1"/>
     <sheet name="municipios_filter_2" sheetId="2" r:id="rId2"/>
+    <sheet name="municipios" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="447">
   <si>
     <t>villa nueva</t>
   </si>
@@ -1364,6 +1365,9 @@
   </si>
   <si>
     <t>destiny sky homes</t>
+  </si>
+  <si>
+    <t>municipios_list</t>
   </si>
 </sst>
 </file>
@@ -1967,8 +1971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18DDAB0F-6443-45E4-9715-DF6063DE65A5}">
   <dimension ref="A1:C419"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A389" zoomScale="87" workbookViewId="0">
-      <selection activeCell="A396" sqref="A396"/>
+    <sheetView topLeftCell="A389" zoomScale="87" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B419"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6412,4 +6416,112 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F329B12-3E83-49AC-BB4B-5E9E77FD3FB6}">
+  <dimension ref="A1:A18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A18">
+    <sortCondition ref="A2:A18"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>